<commit_message>
write results to reports directory
</commit_message>
<xml_diff>
--- a/src/main/resources/accreditation-tests.xlsx
+++ b/src/main/resources/accreditation-tests.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2066" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="344">
   <si>
     <t xml:space="preserve">Test No</t>
   </si>
@@ -1408,177 +1408,6 @@
   <si>
     <t xml:space="preserve">PAD
 CDF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Three Journey Booking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Luton Airport Parkway
-2. Southampton Airport (Parkway)
-3. London Terminals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3645
-5922
-1072</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1. Chesterfield
-2. Basingstoke
-3. Preston
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">*** cannot find an Advance ticket for the London to Preston Journey ***</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">6615
-5520
-2753</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not Via London
-Any Permitted
-Avanti West Coast &amp; Connections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00700
-00000
-00452</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No
-No
-No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/04/2020
-11/04/2020
-14/04/2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10:28
-15:27
-10:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/04/2020
-N/A
-N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12:26
-N/A
-N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0
-1
-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1
-0
-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A
-N/A
-N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Super Off Peak Return
-Super Off Peak Day Single
-Advance Single First</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSR
-FSA
-V1S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BSO
-???
-SFS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CJ
-UL
-VA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33.40
-£17.40
-£45.75</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="6"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Journey 3
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">STP
-STP
-EUS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="6"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Journey 3
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">NOT
-SHF
-GLC</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Sleeper Supplement</t>
@@ -1907,7 +1736,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="hh:mm"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1950,14 +1779,6 @@
       <u val="single"/>
       <sz val="9"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2101,7 +1922,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2213,14 +2034,14 @@
   <dimension ref="A1:AE158"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" activeCellId="1" sqref="90:90 D4"/>
+      <selection pane="bottomRight" activeCell="B90" activeCellId="0" sqref="B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
@@ -2234,8 +2055,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="6.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="5.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.1"/>
@@ -7168,85 +6989,33 @@
       <c r="AD89" s="7"/>
       <c r="AE89" s="7"/>
     </row>
-    <row r="90" s="12" customFormat="true" ht="93.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="7" t="n">
-        <v>3089</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="G90" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="I90" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="J90" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="K90" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="L90" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="M90" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="N90" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="O90" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="P90" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q90" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="R90" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="S90" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="T90" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="U90" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="V90" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="W90" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="X90" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="Y90" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="Z90" s="13" t="s">
-        <v>345</v>
-      </c>
+    <row r="90" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="7"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7"/>
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="9"/>
+      <c r="O90" s="10"/>
+      <c r="P90" s="7"/>
+      <c r="Q90" s="7"/>
+      <c r="R90" s="7"/>
+      <c r="S90" s="7"/>
+      <c r="T90" s="7"/>
+      <c r="U90" s="7"/>
+      <c r="V90" s="7"/>
+      <c r="W90" s="7"/>
+      <c r="X90" s="11"/>
+      <c r="Y90" s="13"/>
+      <c r="Z90" s="13"/>
       <c r="AA90" s="7"/>
       <c r="AB90" s="7"/>
       <c r="AC90" s="7"/>
@@ -7261,7 +7030,7 @@
         <v>127</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>346</v>
+        <v>324</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
@@ -8857,10 +8626,10 @@
   <dimension ref="A1:AD158"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="90:90 D3"/>
+      <selection pane="topLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.26"/>
@@ -8874,8 +8643,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="6.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="5.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.1"/>
@@ -8892,7 +8661,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>347</v>
+        <v>325</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -8981,10 +8750,10 @@
         <v>3001</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>32</v>
@@ -9058,10 +8827,10 @@
         <v>3002</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>44</v>
@@ -9467,10 +9236,10 @@
         <v>3007</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>96</v>
@@ -9629,10 +9398,10 @@
         <v>3009</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>111</v>
@@ -10574,7 +10343,7 @@
         <v>55</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>353</v>
+        <v>331</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>189</v>
@@ -10660,7 +10429,7 @@
         <v>198</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
       <c r="E27" s="7" t="n">
         <v>5886</v>
@@ -11917,10 +11686,10 @@
         <v>3059</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>236</v>
@@ -11929,7 +11698,7 @@
         <v>8610</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="G60" s="7" t="n">
         <v>9149</v>
@@ -12156,7 +11925,7 @@
         <v>55</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>254</v>
@@ -12239,7 +12008,7 @@
         <v>55</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>359</v>
+        <v>337</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>265</v>
@@ -12316,7 +12085,7 @@
         <v>55</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>360</v>
+        <v>338</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>270</v>
@@ -13108,7 +12877,7 @@
         <v>37</v>
       </c>
       <c r="K82" s="7" t="s">
-        <v>361</v>
+        <v>339</v>
       </c>
       <c r="L82" s="9" t="n">
         <v>43936</v>
@@ -13161,7 +12930,7 @@
         <v>30</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>362</v>
+        <v>340</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>173</v>
@@ -13321,7 +13090,7 @@
         <v>55</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>299</v>
@@ -13555,7 +13324,7 @@
         <v>30</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>364</v>
+        <v>342</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>248</v>
@@ -13603,7 +13372,7 @@
         <v>318</v>
       </c>
       <c r="S89" s="7" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="T89" s="7" t="s">
         <v>320</v>
@@ -13628,85 +13397,33 @@
       <c r="AC89" s="7"/>
       <c r="AD89" s="7"/>
     </row>
-    <row r="90" s="12" customFormat="true" ht="93.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="7" t="n">
-        <v>3089</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="G90" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="I90" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="J90" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="K90" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="L90" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="M90" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="N90" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="O90" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="P90" s="7" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q90" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="R90" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="S90" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="T90" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="U90" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="V90" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="W90" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="X90" s="11" t="s">
-        <v>343</v>
-      </c>
-      <c r="Y90" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="Z90" s="13" t="s">
-        <v>345</v>
-      </c>
+    <row r="90" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+      <c r="I90" s="7"/>
+      <c r="J90" s="7"/>
+      <c r="K90" s="7"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="9"/>
+      <c r="O90" s="10"/>
+      <c r="P90" s="7"/>
+      <c r="Q90" s="7"/>
+      <c r="R90" s="7"/>
+      <c r="S90" s="7"/>
+      <c r="T90" s="7"/>
+      <c r="U90" s="7"/>
+      <c r="V90" s="7"/>
+      <c r="W90" s="7"/>
+      <c r="X90" s="11"/>
+      <c r="Y90" s="13"/>
+      <c r="Z90" s="13"/>
       <c r="AB90" s="7"/>
       <c r="AC90" s="7"/>
       <c r="AD90" s="7"/>
@@ -13719,7 +13436,7 @@
         <v>127</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>346</v>
+        <v>324</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
@@ -14741,11 +14458,11 @@
   </sheetPr>
   <dimension ref="A1:AD158"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H90" activeCellId="0" sqref="90:90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H90" activeCellId="0" sqref="H90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.26"/>
@@ -14759,8 +14476,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="6.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="5.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.1"/>
@@ -14777,7 +14494,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>347</v>
+        <v>325</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -14867,10 +14584,10 @@
         <v>3001</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>32</v>
@@ -14945,10 +14662,10 @@
         <v>3002</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>44</v>
@@ -15359,10 +15076,10 @@
         <v>3007</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>96</v>
@@ -15523,10 +15240,10 @@
         <v>3009</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>111</v>
@@ -16484,7 +16201,7 @@
         <v>55</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>353</v>
+        <v>331</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>189</v>
@@ -16571,7 +16288,7 @@
         <v>198</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
       <c r="E27" s="7" t="n">
         <v>5886</v>
@@ -17861,10 +17578,10 @@
         <v>3059</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>236</v>
@@ -17873,7 +17590,7 @@
         <v>8610</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
       <c r="G60" s="7" t="n">
         <v>9149</v>
@@ -18104,7 +17821,7 @@
         <v>55</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>254</v>
@@ -18188,7 +17905,7 @@
         <v>55</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>359</v>
+        <v>337</v>
       </c>
       <c r="D65" s="7" t="s">
         <v>265</v>
@@ -18266,7 +17983,7 @@
         <v>55</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>360</v>
+        <v>338</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>270</v>
@@ -19074,7 +18791,7 @@
         <v>37</v>
       </c>
       <c r="K82" s="7" t="s">
-        <v>361</v>
+        <v>339</v>
       </c>
       <c r="L82" s="9" t="n">
         <v>43936</v>
@@ -19128,7 +18845,7 @@
         <v>30</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>362</v>
+        <v>340</v>
       </c>
       <c r="D83" s="7" t="s">
         <v>173</v>
@@ -19290,7 +19007,7 @@
         <v>55</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="D85" s="7" t="s">
         <v>299</v>
@@ -19530,7 +19247,7 @@
         <v>30</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>364</v>
+        <v>342</v>
       </c>
       <c r="D89" s="7" t="s">
         <v>248</v>
@@ -19578,7 +19295,7 @@
         <v>318</v>
       </c>
       <c r="S89" s="7" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="T89" s="7" t="s">
         <v>320</v>
@@ -19644,7 +19361,7 @@
         <v>127</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>346</v>
+        <v>324</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>

</xml_diff>